<commit_message>
Commit with United Russia data
</commit_message>
<xml_diff>
--- a/raw-data/ldprkprf.xlsx
+++ b/raw-data/ldprkprf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dshap\Documents\GOV-1006\levada\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E791B4D-936B-4166-85AD-9EBD5556AE40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D7FFD2-7D52-4EC4-93D2-EF98F656A973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{07D39F21-60F5-43E8-B19A-88ECFDC68B7D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Percent</t>
+  </si>
+  <si>
+    <t>United Russia</t>
   </si>
 </sst>
 </file>
@@ -409,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4DE7D8E-BAAC-4F48-ABAE-F9A601838B09}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -582,6 +585,83 @@
         <v>9</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>42583</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>43070</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>43313</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>43647</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>43800</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>43862</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>